<commit_message>
subPC 4ch_circular_10cm test eval
</commit_message>
<xml_diff>
--- a/RESULT/evaluation/subset_DEMAND_hoth_10dB_5sec.xlsx
+++ b/RESULT/evaluation/subset_DEMAND_hoth_10dB_5sec.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -840,28 +840,392 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="0" t="inlineStr">
         <is>
           <t>C:\Users\kataoka-lab\Desktop\sound_data\evaluation\sebset_DEMAND_hoth_1010dB_05sec_4ch_3cm\Left\noise_only.csv</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" s="0" t="n">
         <v>1.400322920084</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="0" t="n">
         <v>0.5057229784940992</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="0" t="n">
         <v>-0.005927371792495251</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" s="0" t="inlineStr">
         <is>
           <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\sebset_DEMAND_hoth_1010dB_05sec_4ch_3cm\Left\test\clean</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="0" t="inlineStr">
         <is>
           <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/sebset_DEMAND_hoth_1010dB_05sec_2ch_3cm_Dtype/Left/noise_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Right\noise_only.csv</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>3.555207598209381</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.9829049305704268</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>33.32115936279297</v>
+      </c>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Right\test\clean</t>
+        </is>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/Right/noise_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontRight\noise_only.csv</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>3.662087273597717</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.9853239165057607</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>33.90171051025391</v>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontRight\test\clean</t>
+        </is>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/FrontRight/noise_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Front\noise_only.csv</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>2.170329254865647</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.903891390591925</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>14.7094898223877</v>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Front\test\clean</t>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/Front/noise_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontLeft\noise_only.csv</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>3.679636192321778</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.9864447880212298</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>33.60507965087891</v>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontLeft\test\clean</t>
+        </is>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/FrontLeft/noise_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Left\noise_only.csv</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>3.398727691173554</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.9825341801258716</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>31.5970344543457</v>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Left\test\clean</t>
+        </is>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/Left/noise_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Right\noise_reverbe.csv</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2.303643715381622</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.942897948267561</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>19.03293228149414</v>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Right\test\clean</t>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/Right/noise_reverbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontRight\noise_reverbe.csv</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2.62207989692688</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.9608179637329928</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>21.1391773223877</v>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontRight\test\clean</t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/FrontRight/noise_reverbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontRight\reverbe_only.csv</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>3.079035294055939</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0.9805201789132024</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>21.89427185058594</v>
+      </c>
+      <c r="E22" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontRight\test\clean</t>
+        </is>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/FrontRight/reverbe_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Front\noise_reverbe.csv</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>1.692980843782425</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>0.907805576066866</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>14.99407958984375</v>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Front\test\clean</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/Front/noise_reverbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Front\reverbe_only.csv</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2.923302006721497</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>0.9756118876948369</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>21.40922546386719</v>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Front\test\clean</t>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/Front/reverbe_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontLeft\noise_reverbe.csv</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2.540942287445068</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0.9593165930115036</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>20.86977577209473</v>
+      </c>
+      <c r="E25" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontLeft\test\clean</t>
+        </is>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/FrontLeft/noise_reverbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontLeft\reverbe_only.csv</t>
+        </is>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3.053740119934082</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0.9807686714588723</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>21.64970588684082</v>
+      </c>
+      <c r="E26" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\FrontLeft\test\clean</t>
+        </is>
+      </c>
+      <c r="F26" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/FrontLeft/reverbe_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Left\noise_reverbe.csv</t>
+        </is>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2.104562246799469</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0.945898200075469</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>19.58468627929688</v>
+      </c>
+      <c r="E27" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Left\test\clean</t>
+        </is>
+      </c>
+      <c r="F27" s="0" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/Left/noise_reverbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\evaluation\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Left\reverbe_only.csv</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2.900625514984131</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.9768721380945248</v>
+      </c>
+      <c r="D28" t="n">
+        <v>21.19450759887695</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\mix_data\subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm\Left\test\clean</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>C:\Users\kataoka-lab\Desktop\sound_data\RESULT\output_wav/subset_DEMAND_hoth_1010dB_05sec_4ch_circular_10cm_Dtype/Left/reverbe_only</t>
         </is>
       </c>
     </row>

</xml_diff>